<commit_message>
Update spreadsheets and trace scripts for pl_clk_1 = 187.5MHz.
</commit_message>
<xml_diff>
--- a/system/clocks_zcu102.xlsx
+++ b/system/clocks_zcu102.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macaraeg1\Projects\comp\repositories\lime_axi_delayv\system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3325AF-7BD6-4BA6-AE9B-C8DE80AE8333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463A8796-A5B6-4E13-A2F4-362B378B386D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="340" windowWidth="13570" windowHeight="20680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10" yWindow="0" windowWidth="19870" windowHeight="20950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -859,7 +859,7 @@
   <dimension ref="A1:K108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1468,26 +1468,26 @@
         <v>87</v>
       </c>
       <c r="C28" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D28" s="3">
         <v>1</v>
       </c>
       <c r="E28" s="7">
         <f>VLOOKUP($B28,$A$11:$F$16,5,FALSE)/$C28/$D28</f>
-        <v>249.97499999999999</v>
+        <v>187.48124999999999</v>
       </c>
       <c r="F28" s="4">
         <f t="shared" si="4"/>
-        <v>4.0004000400040001</v>
+        <v>5.3338667200053349</v>
       </c>
       <c r="G28" s="9">
         <f t="shared" si="5"/>
-        <v>4999.5</v>
+        <v>3749.625</v>
       </c>
       <c r="H28" s="9">
         <f t="shared" si="6"/>
-        <v>0.20002000200020001</v>
+        <v>0.26669333600026673</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
@@ -1528,26 +1528,26 @@
         <v>87</v>
       </c>
       <c r="C30" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
       </c>
       <c r="E30" s="7">
         <f t="shared" ref="E30:E32" si="8">VLOOKUP($B30,$A$11:$F$16,5,FALSE)/$C30/$D30</f>
-        <v>249.97499999999999</v>
+        <v>187.48124999999999</v>
       </c>
       <c r="F30" s="4">
         <f t="shared" si="4"/>
-        <v>4.0004000400040001</v>
+        <v>5.3338667200053349</v>
       </c>
       <c r="G30" s="9">
         <f t="shared" si="5"/>
-        <v>4999.5</v>
+        <v>3749.625</v>
       </c>
       <c r="H30" s="9">
         <f t="shared" si="6"/>
-        <v>0.20002000200020001</v>
+        <v>0.26669333600026673</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
@@ -1817,19 +1817,19 @@
       </c>
       <c r="E41" s="12">
         <f t="shared" si="9"/>
-        <v>249.97499999999999</v>
+        <v>187.48124999999999</v>
       </c>
       <c r="F41" s="4">
         <f>1/$E41*1000</f>
-        <v>4.0004000400040001</v>
+        <v>5.3338667200053349</v>
       </c>
       <c r="G41" s="9">
         <f>$E41*$B$3</f>
-        <v>4999.5</v>
+        <v>3749.625</v>
       </c>
       <c r="H41" s="9">
         <f t="shared" si="10"/>
-        <v>0.20002000200020001</v>
+        <v>0.26669333600026673</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
@@ -2118,19 +2118,19 @@
       </c>
       <c r="E53" s="9">
         <f t="shared" si="11"/>
-        <v>3999.6</v>
+        <v>2999.7</v>
       </c>
       <c r="F53" s="9">
         <f t="shared" si="12"/>
-        <v>4.0004000400040001</v>
+        <v>5.3338667200053349</v>
       </c>
       <c r="G53" s="12">
         <f t="shared" si="13"/>
-        <v>79992</v>
+        <v>59994</v>
       </c>
       <c r="H53" s="12">
         <f t="shared" si="14"/>
-        <v>0.20002000200020001</v>
+        <v>0.26669333600026673</v>
       </c>
       <c r="J53" t="s">
         <v>35</v>
@@ -2151,19 +2151,19 @@
       </c>
       <c r="E54" s="9">
         <f t="shared" si="11"/>
-        <v>1999.8</v>
+        <v>1499.85</v>
       </c>
       <c r="F54" s="9">
         <f t="shared" si="12"/>
-        <v>4.0004000400040001</v>
+        <v>5.3338667200053349</v>
       </c>
       <c r="G54" s="9">
         <f t="shared" si="13"/>
-        <v>39996</v>
+        <v>29997</v>
       </c>
       <c r="H54" s="9">
         <f t="shared" si="14"/>
-        <v>0.20002000200020001</v>
+        <v>0.26669333600026673</v>
       </c>
       <c r="J54" t="s">
         <v>36</v>
@@ -2184,19 +2184,19 @@
       </c>
       <c r="E55" s="9">
         <f t="shared" si="11"/>
-        <v>15998.4</v>
+        <v>11998.8</v>
       </c>
       <c r="F55" s="9">
         <f t="shared" si="12"/>
-        <v>4.0004000400040001</v>
+        <v>5.3338667200053349</v>
       </c>
       <c r="G55" s="9">
         <f t="shared" si="13"/>
-        <v>319968</v>
+        <v>239976</v>
       </c>
       <c r="H55" s="9">
         <f t="shared" si="14"/>
-        <v>0.20002000200020001</v>
+        <v>0.26669333600026673</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
@@ -2425,27 +2425,27 @@
       </c>
       <c r="D70">
         <f>($B$62+$B$61)*ROUND($B$3/VLOOKUP($B70,$A$20:$F$35,6,FALSE),0)-$C70</f>
-        <v>128</v>
+        <v>92</v>
       </c>
       <c r="E70" s="12">
         <f>$C70*VLOOKUP($B70,$A$20:$F$35,6,FALSE)</f>
-        <v>208.020802080208</v>
+        <v>277.36106944027739</v>
       </c>
       <c r="F70" s="12">
         <f>$D70*VLOOKUP($B70,$A$20:$F$35,6,FALSE)</f>
-        <v>512.05120512051201</v>
+        <v>490.71573824049079</v>
       </c>
       <c r="G70" s="4">
         <f>$E70/$B$3</f>
-        <v>10.4010401040104</v>
+        <v>13.86805347201387</v>
       </c>
       <c r="H70" s="4">
         <f>$F70/$B$3</f>
-        <v>25.602560256025601</v>
+        <v>24.535786912024541</v>
       </c>
       <c r="I70" s="4">
         <f>$G70+$H70</f>
-        <v>36.003600360036003</v>
+        <v>38.403840384038411</v>
       </c>
       <c r="K70" t="s">
         <v>75</v>
@@ -2463,27 +2463,27 @@
       </c>
       <c r="D71">
         <f>($B$63+$B$61)*ROUND($B$3/VLOOKUP($B71,$A$20:$F$35,6,FALSE),0)-$C71</f>
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="E71" s="12">
         <f t="shared" ref="E71:E77" si="15">$C71*VLOOKUP($B71,$A$20:$F$35,6,FALSE)</f>
-        <v>276.02760276027601</v>
+        <v>368.03680368036811</v>
       </c>
       <c r="F71" s="12">
         <f t="shared" ref="F71:F77" si="16">$D71*VLOOKUP($B71,$A$20:$F$35,6,FALSE)</f>
-        <v>444.044404440444</v>
+        <v>400.04000400040013</v>
       </c>
       <c r="G71" s="4">
         <f t="shared" ref="G71:G77" si="17">$E71/$B$3</f>
-        <v>13.801380138013801</v>
+        <v>18.401840184018404</v>
       </c>
       <c r="H71" s="4">
         <f t="shared" ref="H71:H77" si="18">$F71/$B$3</f>
-        <v>22.202220222022198</v>
+        <v>20.002000200020007</v>
       </c>
       <c r="I71" s="4">
         <f t="shared" ref="I71:I77" si="19">$G71+$H71</f>
-        <v>36.003600360036003</v>
+        <v>38.403840384038411</v>
       </c>
       <c r="K71" t="s">
         <v>76</v>
@@ -2501,27 +2501,27 @@
       </c>
       <c r="D72">
         <f>($B$64+$B$66+$B$61)*ROUND($B$3/VLOOKUP($B72,$A$20:$F$35,6,FALSE),0)-$C72</f>
-        <v>478</v>
+        <v>372</v>
       </c>
       <c r="E72" s="12">
         <f t="shared" si="15"/>
-        <v>208.020802080208</v>
+        <v>277.36106944027739</v>
       </c>
       <c r="F72" s="12">
         <f t="shared" si="16"/>
-        <v>1912.1912191219121</v>
+        <v>1984.1984198419846</v>
       </c>
       <c r="G72" s="4">
         <f t="shared" si="17"/>
-        <v>10.4010401040104</v>
+        <v>13.86805347201387</v>
       </c>
       <c r="H72" s="4">
         <f t="shared" si="18"/>
-        <v>95.609560956095606</v>
+        <v>99.209920992099228</v>
       </c>
       <c r="I72" s="4">
         <f t="shared" si="19"/>
-        <v>106.01060106010601</v>
+        <v>113.0779744641131</v>
       </c>
       <c r="K72" t="s">
         <v>77</v>
@@ -2539,27 +2539,27 @@
       </c>
       <c r="D73">
         <f>($B$65+$B$67+$B$61)*ROUND($B$3/VLOOKUP($B73,$A$20:$F$35,6,FALSE),0)-$C73</f>
-        <v>356</v>
+        <v>271</v>
       </c>
       <c r="E73" s="12">
         <f t="shared" si="15"/>
-        <v>276.02760276027601</v>
+        <v>368.03680368036811</v>
       </c>
       <c r="F73" s="12">
         <f t="shared" si="16"/>
-        <v>1424.1424142414239</v>
+        <v>1445.4778811214458</v>
       </c>
       <c r="G73" s="4">
         <f t="shared" si="17"/>
-        <v>13.801380138013801</v>
+        <v>18.401840184018404</v>
       </c>
       <c r="H73" s="4">
         <f t="shared" si="18"/>
-        <v>71.207120712071202</v>
+        <v>72.273894056072294</v>
       </c>
       <c r="I73" s="4">
         <f t="shared" si="19"/>
-        <v>85.008500850084999</v>
+        <v>90.675734240090691</v>
       </c>
       <c r="K73" t="s">
         <v>78</v>
@@ -2577,27 +2577,27 @@
       </c>
       <c r="D74">
         <f>($B$62)*ROUND($B$3/VLOOKUP($B74,$A$20:$F$35,6,FALSE),0)-$C74</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E74" s="12">
         <f t="shared" si="15"/>
-        <v>192.01920192019202</v>
+        <v>256.02560256025606</v>
       </c>
       <c r="F74" s="12">
         <f t="shared" si="16"/>
-        <v>48.004800480048004</v>
+        <v>0</v>
       </c>
       <c r="G74" s="4">
         <f t="shared" si="17"/>
-        <v>9.6009600960096009</v>
+        <v>12.801280128012802</v>
       </c>
       <c r="H74" s="4">
         <f t="shared" si="18"/>
-        <v>2.4002400240024002</v>
+        <v>0</v>
       </c>
       <c r="I74" s="4">
         <f t="shared" si="19"/>
-        <v>12.001200120012001</v>
+        <v>12.801280128012802</v>
       </c>
       <c r="K74" t="s">
         <v>79</v>
@@ -2615,27 +2615,27 @@
       </c>
       <c r="D75">
         <f>($B$63)*ROUND($B$3/VLOOKUP($B75,$A$20:$F$35,6,FALSE),0)-$C75</f>
-        <v>-6</v>
+        <v>-18</v>
       </c>
       <c r="E75" s="12">
         <f t="shared" si="15"/>
-        <v>264.026402640264</v>
+        <v>352.03520352035213</v>
       </c>
       <c r="F75" s="12">
         <f t="shared" si="16"/>
-        <v>-24.002400240024002</v>
+        <v>-96.009600960096023</v>
       </c>
       <c r="G75" s="4">
         <f t="shared" si="17"/>
-        <v>13.201320132013199</v>
+        <v>17.601760176017606</v>
       </c>
       <c r="H75" s="4">
         <f t="shared" si="18"/>
-        <v>-1.2001200120012001</v>
+        <v>-4.8004800480048013</v>
       </c>
       <c r="I75" s="4">
         <f t="shared" si="19"/>
-        <v>12.001200120011999</v>
+        <v>12.801280128012806</v>
       </c>
       <c r="K75" t="s">
         <v>80</v>
@@ -2653,27 +2653,27 @@
       </c>
       <c r="D76">
         <f>($B$64+$B$66)*ROUND($B$3/VLOOKUP($B76,$A$20:$F$35,6,FALSE),0)-$C76</f>
-        <v>362</v>
+        <v>280</v>
       </c>
       <c r="E76" s="12">
         <f t="shared" si="15"/>
-        <v>192.01920192019202</v>
+        <v>256.02560256025606</v>
       </c>
       <c r="F76" s="12">
         <f t="shared" si="16"/>
-        <v>1448.1448144814481</v>
+        <v>1493.4826816014938</v>
       </c>
       <c r="G76" s="4">
         <f t="shared" si="17"/>
-        <v>9.6009600960096009</v>
+        <v>12.801280128012802</v>
       </c>
       <c r="H76" s="4">
         <f t="shared" si="18"/>
-        <v>72.407240724072409</v>
+        <v>74.674134080074694</v>
       </c>
       <c r="I76" s="4">
         <f t="shared" si="19"/>
-        <v>82.00820082008201</v>
+        <v>87.4754142080875</v>
       </c>
       <c r="K76" t="s">
         <v>81</v>
@@ -2691,27 +2691,27 @@
       </c>
       <c r="D77">
         <f>($B$65+$B$67)*ROUND($B$3/VLOOKUP($B77,$A$20:$F$35,6,FALSE),0)-$C77</f>
-        <v>239</v>
+        <v>178</v>
       </c>
       <c r="E77" s="12">
         <f t="shared" si="15"/>
-        <v>264.026402640264</v>
+        <v>352.03520352035213</v>
       </c>
       <c r="F77" s="12">
         <f t="shared" si="16"/>
-        <v>956.09560956095606</v>
+        <v>949.42827616094962</v>
       </c>
       <c r="G77" s="4">
         <f t="shared" si="17"/>
-        <v>13.201320132013199</v>
+        <v>17.601760176017606</v>
       </c>
       <c r="H77" s="4">
         <f t="shared" si="18"/>
-        <v>47.804780478047803</v>
+        <v>47.47141380804748</v>
       </c>
       <c r="I77" s="4">
         <f t="shared" si="19"/>
-        <v>61.006100610061004</v>
+        <v>65.073173984065079</v>
       </c>
       <c r="K77" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
Update files for timing calibration and performance testing.
</commit_message>
<xml_diff>
--- a/system/clocks_zcu102.xlsx
+++ b/system/clocks_zcu102.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macaraeg1\Projects\comp\repositories\lime_axi_delayv\system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463A8796-A5B6-4E13-A2F4-362B378B386D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600F1BCE-1DE0-48FF-A7CE-2AA79AF511A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10" yWindow="0" windowWidth="19870" windowHeight="20950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -858,8 +858,8 @@
   </sheetPr>
   <dimension ref="A1:K108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>